<commit_message>
items added. need details.
</commit_message>
<xml_diff>
--- a/src/assets/art/bartending/bartendingsheet.xlsx
+++ b/src/assets/art/bartending/bartendingsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="224">
   <si>
     <t>Recipe</t>
   </si>
@@ -354,9 +354,6 @@
     <t>done</t>
   </si>
   <si>
-    <t>waiting</t>
-  </si>
-  <si>
     <t>in prog.</t>
   </si>
   <si>
@@ -690,10 +687,10 @@
     <t>Equati:</t>
   </si>
   <si>
-    <t>(level/10)/second makes for a good balance, consider boosting the beginning</t>
-  </si>
-  <si>
     <t>-50</t>
+  </si>
+  <si>
+    <t>(level/10)/sec (1.6?)</t>
   </si>
 </sst>
 </file>
@@ -766,97 +763,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="23">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6D6D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6D6D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dashDot">
-          <color auto="1"/>
-        </left>
-        <right style="dashDot">
-          <color auto="1"/>
-        </right>
-        <top style="dashDot">
-          <color auto="1"/>
-        </top>
-        <bottom style="dashDot">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1085,6 +991,97 @@
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6D6D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6D6D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dashDot">
+          <color auto="1"/>
+        </left>
+        <right style="dashDot">
+          <color auto="1"/>
+        </right>
+        <top style="dashDot">
+          <color auto="1"/>
+        </top>
+        <bottom style="dashDot">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1102,22 +1099,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J45" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J45" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:J45"/>
   <sortState ref="A2:I45">
     <sortCondition ref="H1:H45"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" name="Unlock Lvl." dataDxfId="14"/>
-    <tableColumn id="2" name="Recipe" dataDxfId="12"/>
-    <tableColumn id="3" name="Requires" dataDxfId="13"/>
-    <tableColumn id="4" name="Produces" dataDxfId="20"/>
-    <tableColumn id="5" name="Time" dataDxfId="19"/>
-    <tableColumn id="6" name="XP" dataDxfId="18"/>
-    <tableColumn id="7" name="Sell Value" dataDxfId="17"/>
-    <tableColumn id="8" name="&quot;Tier&quot;" dataDxfId="16"/>
-    <tableColumn id="9" name="Stats" dataDxfId="15"/>
-    <tableColumn id="10" name="Notes" dataDxfId="11"/>
+    <tableColumn id="1" name="Unlock Lvl." dataDxfId="9"/>
+    <tableColumn id="2" name="Recipe" dataDxfId="8"/>
+    <tableColumn id="3" name="Requires" dataDxfId="7"/>
+    <tableColumn id="4" name="Produces" dataDxfId="6"/>
+    <tableColumn id="5" name="Time" dataDxfId="5"/>
+    <tableColumn id="6" name="XP" dataDxfId="4"/>
+    <tableColumn id="7" name="Sell Value" dataDxfId="3"/>
+    <tableColumn id="8" name="&quot;Tier&quot;" dataDxfId="2"/>
+    <tableColumn id="9" name="Stats" dataDxfId="1"/>
+    <tableColumn id="10" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1412,10 +1409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="9750" topLeftCell="A46" activePane="bottomLeft"/>
-      <selection activeCell="I44" sqref="I44"/>
-      <selection pane="bottomLeft" activeCell="I48" sqref="I48"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1435,7 +1430,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1459,7 +1454,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>10</v>
@@ -1508,7 +1503,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
@@ -1621,12 +1616,12 @@
         <v>70</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>14</v>
@@ -1641,7 +1636,7 @@
         <v>107</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>65</v>
@@ -1650,12 +1645,12 @@
         <v>70</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>15</v>
@@ -1670,7 +1665,7 @@
         <v>107</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>66</v>
@@ -1679,7 +1674,7 @@
         <v>70</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1708,7 +1703,7 @@
         <v>70</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1737,7 +1732,7 @@
         <v>70</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1756,6 +1751,9 @@
       <c r="E12" s="2" t="s">
         <v>69</v>
       </c>
+      <c r="F12" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="G12" s="2" t="s">
         <v>102</v>
       </c>
@@ -1780,7 +1778,7 @@
         <v>69</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>65</v>
@@ -1794,7 +1792,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>86</v>
@@ -1803,7 +1801,7 @@
         <v>69</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>65</v>
@@ -1817,7 +1815,7 @@
         <v>29</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>87</v>
@@ -1826,7 +1824,7 @@
         <v>69</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>65</v>
@@ -1840,7 +1838,7 @@
         <v>41</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>98</v>
@@ -1849,7 +1847,7 @@
         <v>69</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>65</v>
@@ -1863,7 +1861,7 @@
         <v>18</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>76</v>
@@ -1872,7 +1870,7 @@
         <v>69</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>68</v>
@@ -1886,7 +1884,7 @@
         <v>34</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>91</v>
@@ -1895,7 +1893,7 @@
         <v>69</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>68</v>
@@ -1903,13 +1901,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>95</v>
@@ -1918,7 +1916,7 @@
         <v>69</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>68</v>
@@ -1926,13 +1924,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>84</v>
@@ -1941,7 +1939,7 @@
         <v>69</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>68</v>
@@ -1949,13 +1947,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>94</v>
@@ -1964,7 +1962,7 @@
         <v>69</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>68</v>
@@ -1972,22 +1970,22 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="E22" s="2" t="s">
         <v>69</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>68</v>
@@ -1995,7 +1993,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>19</v>
@@ -2010,7 +2008,7 @@
         <v>69</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>69</v>
@@ -2018,22 +2016,22 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>69</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>69</v>
@@ -2041,13 +2039,13 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>90</v>
@@ -2056,7 +2054,7 @@
         <v>69</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>69</v>
@@ -2064,13 +2062,13 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>92</v>
@@ -2079,7 +2077,7 @@
         <v>69</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>69</v>
@@ -2087,13 +2085,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>99</v>
@@ -2102,7 +2100,7 @@
         <v>69</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>69</v>
@@ -2110,13 +2108,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>93</v>
@@ -2125,7 +2123,7 @@
         <v>69</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>69</v>
@@ -2133,13 +2131,13 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>83</v>
@@ -2148,7 +2146,7 @@
         <v>69</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>73</v>
@@ -2156,13 +2154,13 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>82</v>
@@ -2171,7 +2169,7 @@
         <v>69</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>73</v>
@@ -2179,13 +2177,13 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>81</v>
@@ -2194,7 +2192,7 @@
         <v>69</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>73</v>
@@ -2202,13 +2200,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>85</v>
@@ -2217,7 +2215,7 @@
         <v>69</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>73</v>
@@ -2225,13 +2223,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>89</v>
@@ -2240,7 +2238,7 @@
         <v>69</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>73</v>
@@ -2248,13 +2246,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>97</v>
@@ -2263,7 +2261,7 @@
         <v>69</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>73</v>
@@ -2271,13 +2269,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>88</v>
@@ -2286,7 +2284,7 @@
         <v>69</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>102</v>
@@ -2294,13 +2292,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>101</v>
@@ -2309,7 +2307,7 @@
         <v>69</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>102</v>
@@ -2317,13 +2315,13 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>179</v>
+        <v>215</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>100</v>
@@ -2332,7 +2330,7 @@
         <v>69</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>102</v>
@@ -2346,7 +2344,7 @@
         <v>39</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>96</v>
@@ -2355,7 +2353,7 @@
         <v>69</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>102</v>
@@ -2363,13 +2361,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>80</v>
@@ -2378,10 +2376,10 @@
         <v>69</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>102</v>
@@ -2395,10 +2393,10 @@
         <v>6</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>223</v>
@@ -2413,6 +2411,9 @@
       </c>
       <c r="G48" s="4">
         <v>0</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
@@ -2436,7 +2437,7 @@
         <v>110</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -2452,7 +2453,7 @@
         <v>110</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -2468,7 +2469,7 @@
         <v>110</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -2484,7 +2485,7 @@
         <v>110</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -2497,14 +2498,14 @@
     </row>
     <row r="54" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C54" s="1"/>
       <c r="F54" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G54" s="4">
         <v>425</v>
@@ -2515,7 +2516,7 @@
         <v>110</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -2531,12 +2532,12 @@
         <v>110</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="F56" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G56" s="4">
         <v>698</v>
@@ -2547,7 +2548,7 @@
         <v>111</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -2560,7 +2561,7 @@
     </row>
     <row r="58" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>63</v>
@@ -2568,7 +2569,7 @@
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="F58" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G58" s="4">
         <v>1047</v>
@@ -2576,15 +2577,15 @@
     </row>
     <row r="59" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="F59" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G59" s="4">
         <v>1255</v>
@@ -2592,7 +2593,7 @@
     </row>
     <row r="60" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>109</v>
@@ -2600,7 +2601,7 @@
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="F60" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G60" s="4">
         <v>1486</v>
@@ -2608,7 +2609,7 @@
     </row>
     <row r="61" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>64</v>
@@ -2616,7 +2617,7 @@
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="F61" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G61" s="4">
         <v>1744</v>
@@ -2624,7 +2625,7 @@
     </row>
     <row r="62" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>62</v>
@@ -2640,15 +2641,15 @@
     </row>
     <row r="63" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="F63" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G63" s="4">
         <v>2351</v>
@@ -2656,15 +2657,15 @@
     </row>
     <row r="64" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="F64" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G64" s="4">
         <v>2705</v>
@@ -2674,7 +2675,7 @@
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="F65" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G65" s="4">
         <v>3098</v>
@@ -2684,7 +2685,7 @@
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="F66" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G66" s="4">
         <v>3534</v>
@@ -2692,7 +2693,7 @@
     </row>
     <row r="67" spans="3:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F67" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G67" s="4">
         <v>4017</v>
@@ -2700,7 +2701,7 @@
     </row>
     <row r="68" spans="3:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F68" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G68" s="4">
         <v>4551</v>
@@ -2708,7 +2709,7 @@
     </row>
     <row r="69" spans="3:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F69" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G69" s="4">
         <v>5142</v>
@@ -2716,7 +2717,7 @@
     </row>
     <row r="70" spans="3:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F70" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G70" s="4">
         <v>5796</v>
@@ -2724,7 +2725,7 @@
     </row>
     <row r="71" spans="3:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F71" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G71" s="4">
         <v>6519</v>
@@ -2740,7 +2741,7 @@
     </row>
     <row r="73" spans="3:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F73" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G73" s="4">
         <v>8203</v>
@@ -2748,7 +2749,7 @@
     </row>
     <row r="74" spans="3:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F74" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G74" s="4">
         <v>9180</v>
@@ -2756,7 +2757,7 @@
     </row>
     <row r="75" spans="3:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F75" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G75" s="4">
         <v>10260</v>
@@ -2764,7 +2765,7 @@
     </row>
     <row r="76" spans="3:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F76" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G76" s="4">
         <v>11453</v>
@@ -2772,7 +2773,7 @@
     </row>
     <row r="77" spans="3:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F77" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G77" s="4">
         <v>12772</v>
@@ -2780,7 +2781,7 @@
     </row>
     <row r="78" spans="3:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F78" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G78" s="4">
         <v>14228</v>
@@ -2788,7 +2789,7 @@
     </row>
     <row r="79" spans="3:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F79" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G79" s="4">
         <v>15837</v>
@@ -2796,7 +2797,7 @@
     </row>
     <row r="80" spans="3:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F80" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G80" s="4">
         <v>17614</v>
@@ -2804,7 +2805,7 @@
     </row>
     <row r="81" spans="6:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F81" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G81" s="4">
         <v>19578</v>
@@ -2812,7 +2813,7 @@
     </row>
     <row r="82" spans="6:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F82" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G82" s="4">
         <v>21746</v>
@@ -2820,7 +2821,7 @@
     </row>
     <row r="83" spans="6:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F83" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G83" s="4">
         <v>24140</v>
@@ -2828,7 +2829,7 @@
     </row>
     <row r="84" spans="6:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F84" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G84" s="4">
         <v>26785</v>
@@ -2836,7 +2837,7 @@
     </row>
     <row r="85" spans="6:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F85" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G85" s="4">
         <v>29705</v>
@@ -2844,7 +2845,7 @@
     </row>
     <row r="86" spans="6:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F86" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G86" s="4">
         <v>32930</v>
@@ -2852,7 +2853,7 @@
     </row>
     <row r="87" spans="6:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F87" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G87" s="4">
         <v>36492</v>
@@ -2860,7 +2861,7 @@
     </row>
     <row r="88" spans="6:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F88" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G88" s="4">
         <v>40425</v>
@@ -2868,7 +2869,7 @@
     </row>
     <row r="89" spans="6:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F89" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G89" s="4">
         <v>44767</v>
@@ -2876,7 +2877,7 @@
     </row>
     <row r="90" spans="6:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F90" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G90" s="4">
         <v>49563</v>
@@ -2884,7 +2885,7 @@
     </row>
     <row r="91" spans="6:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F91" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G91" s="4">
         <v>54858</v>
@@ -2892,7 +2893,7 @@
     </row>
     <row r="92" spans="6:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F92" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G92" s="4">
         <v>60705</v>
@@ -2900,7 +2901,7 @@
     </row>
     <row r="93" spans="6:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F93" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G93" s="4">
         <v>67161</v>
@@ -2908,7 +2909,7 @@
     </row>
     <row r="94" spans="6:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F94" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G94" s="4">
         <v>74289</v>
@@ -2916,7 +2917,7 @@
     </row>
     <row r="95" spans="6:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F95" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G95" s="4">
         <v>82160</v>
@@ -2924,7 +2925,7 @@
     </row>
     <row r="96" spans="6:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F96" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G96" s="4">
         <v>90851</v>
@@ -2932,7 +2933,7 @@
     </row>
     <row r="97" spans="6:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="F97" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G97" s="4">
         <v>100447</v>
@@ -2940,49 +2941,49 @@
     </row>
     <row r="99" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F99" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="G99" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>221</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A42:H45 A38:A41 B38:H39 A2:H37">
-    <cfRule type="containsBlanks" dxfId="10" priority="14">
+    <cfRule type="containsBlanks" dxfId="22" priority="14">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:A58 A60:A84">
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="on hold">
+    <cfRule type="containsText" dxfId="21" priority="6" operator="containsText" text="on hold">
       <formula>NOT(ISERROR(SEARCH("on hold",A49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="not begun">
+    <cfRule type="containsText" dxfId="20" priority="7" operator="containsText" text="not begun">
       <formula>NOT(ISERROR(SEARCH("not begun",A49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="waiting">
+    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="waiting">
       <formula>NOT(ISERROR(SEARCH("waiting",A49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="in prog.">
+    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="in prog.">
       <formula>NOT(ISERROR(SEARCH("in prog.",A49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="done">
+    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="done">
       <formula>NOT(ISERROR(SEARCH("done",A49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="on hold">
+    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="on hold">
       <formula>NOT(ISERROR(SEARCH("on hold",A59)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="not begun">
+    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="not begun">
       <formula>NOT(ISERROR(SEARCH("not begun",A59)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="waiting">
+    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="waiting">
       <formula>NOT(ISERROR(SEARCH("waiting",A59)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="in prog.">
+    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="in prog.">
       <formula>NOT(ISERROR(SEARCH("in prog.",A59)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="done">
+    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="done">
       <formula>NOT(ISERROR(SEARCH("done",A59)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>